<commit_message>
Fixed well fields in integration test.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{27F04A51-68CD-9847-BAF1-974E5DBD34A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{019426B7-9FB9-F248-8B03-F0271568274D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="509">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -730,12 +730,6 @@
     <t>cell_suspension.biomaterial_core.genotype</t>
   </si>
   <si>
-    <t>cell_suspension.biomaterial_core.karyotype</t>
-  </si>
-  <si>
-    <t>cell_suspension.biomaterial_core.supplementary_files</t>
-  </si>
-  <si>
     <t>cell_suspension.biomaterial_core.biosd_biomaterial</t>
   </si>
   <si>
@@ -958,48 +952,15 @@
     <t>An ID for the plate that the well is located on.</t>
   </si>
   <si>
-    <t>Well plate ID</t>
-  </si>
-  <si>
-    <t>sequence_file.smartseq2.plate_id</t>
-  </si>
-  <si>
     <t>A name for the well. Should be unique for the plate</t>
   </si>
   <si>
-    <t>Well name</t>
-  </si>
-  <si>
-    <t>sequence_file.smartseq2.well_name</t>
-  </si>
-  <si>
-    <t>Well row in plate.</t>
-  </si>
-  <si>
-    <t>Well row</t>
-  </si>
-  <si>
-    <t>sequence_file.smartseq2.well_row</t>
-  </si>
-  <si>
-    <t>Well column in plate.</t>
-  </si>
-  <si>
-    <t>Well column</t>
-  </si>
-  <si>
-    <t>sequence_file.smartseq2.well_column</t>
-  </si>
-  <si>
     <t>Note on how good cell looks if imaged in well before sequencing.</t>
   </si>
   <si>
     <t>Cell quality</t>
   </si>
   <si>
-    <t>sequence_file.smartseq2.cell_quality</t>
-  </si>
-  <si>
     <t>library_preparation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -1580,6 +1541,21 @@
   </si>
   <si>
     <t>UBERON:0001871</t>
+  </si>
+  <si>
+    <t>Plate ID</t>
+  </si>
+  <si>
+    <t>Well ID</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.plate_id</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.well_id</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.cell_quality</t>
   </si>
 </sst>
 </file>
@@ -1628,18 +1604,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1660,13 +1630,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2056,29 +2025,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2098,7 +2067,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2122,20 +2091,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C6" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -2147,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:L6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2172,146 +2141,146 @@
         <v>224</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>337</v>
+      <c r="B2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>462</v>
+        <v>446</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>449</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>470</v>
+        <v>456</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="J3" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="B4" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4" t="s">
+        <v>442</v>
+      </c>
+      <c r="E4" t="s">
+        <v>443</v>
+      </c>
+      <c r="F4" t="s">
+        <v>444</v>
+      </c>
+      <c r="G4" t="s">
+        <v>446</v>
+      </c>
+      <c r="H4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I4" t="s">
+        <v>450</v>
+      </c>
+      <c r="J4" t="s">
         <v>454</v>
       </c>
-      <c r="D4" t="s">
-        <v>455</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>456</v>
       </c>
-      <c r="F4" t="s">
+      <c r="L4" t="s">
         <v>457</v>
       </c>
-      <c r="G4" t="s">
-        <v>459</v>
-      </c>
-      <c r="H4" t="s">
-        <v>460</v>
-      </c>
-      <c r="I4" t="s">
-        <v>463</v>
-      </c>
-      <c r="J4" t="s">
-        <v>467</v>
-      </c>
-      <c r="K4" t="s">
-        <v>469</v>
-      </c>
-      <c r="L4" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>480</v>
+      </c>
+      <c r="G6" t="s">
+        <v>481</v>
+      </c>
+      <c r="J6" t="s">
+        <v>453</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="G6" t="s">
+      <c r="L6" s="7" t="s">
         <v>494</v>
-      </c>
-      <c r="J6" t="s">
-        <v>466</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -2365,30 +2334,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>513</v>
+      <c r="H2" s="2" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2422,26 +2391,26 @@
         <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="D6" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="H6" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -2649,146 +2618,146 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO2" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AP2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AS2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AT2" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AU2" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2935,32 +2904,32 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B6" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="V6" t="s">
+        <v>453</v>
+      </c>
+      <c r="Y6" t="s">
         <v>466</v>
       </c>
-      <c r="Y6" t="s">
-        <v>479</v>
-      </c>
       <c r="AQ6" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="AR6" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -2972,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3118,110 +3087,110 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="T2" s="3" t="s">
+      <c r="R2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="2" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3283,10 +3252,10 @@
         <v>191</v>
       </c>
       <c r="R4" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="S4" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="T4" t="s">
         <v>192</v>
@@ -3337,44 +3306,44 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="B6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C6" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
       <c r="F6" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="H6" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="I6" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="J6" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="K6" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="R6" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="V6" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -3385,10 +3354,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3397,34 +3366,32 @@
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="51.6640625" customWidth="1"/>
-    <col min="14" max="14" width="55.6640625" customWidth="1"/>
-    <col min="15" max="15" width="68.6640625" customWidth="1"/>
-    <col min="16" max="16" width="21.6640625" customWidth="1"/>
-    <col min="17" max="17" width="67.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="21" width="25.6640625" customWidth="1"/>
-    <col min="22" max="22" width="26.6640625" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" customWidth="1"/>
-    <col min="24" max="24" width="34.6640625" customWidth="1"/>
-    <col min="25" max="25" width="38.6640625" customWidth="1"/>
-    <col min="26" max="26" width="39.6640625" customWidth="1"/>
-    <col min="27" max="27" width="43.6640625" customWidth="1"/>
-    <col min="28" max="28" width="26.6640625" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" customWidth="1"/>
-    <col min="30" max="31" width="11.6640625" customWidth="1"/>
+    <col min="6" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="51.6640625" customWidth="1"/>
+    <col min="15" max="15" width="55.6640625" customWidth="1"/>
+    <col min="16" max="16" width="68.6640625" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" customWidth="1"/>
+    <col min="18" max="18" width="67.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="25.6640625" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" customWidth="1"/>
+    <col min="25" max="25" width="34.6640625" customWidth="1"/>
+    <col min="26" max="26" width="38.6640625" customWidth="1"/>
+    <col min="27" max="27" width="39.6640625" customWidth="1"/>
+    <col min="28" max="28" width="43.6640625" customWidth="1"/>
+    <col min="29" max="29" width="26.6640625" customWidth="1"/>
+    <col min="30" max="30" width="10.6640625" customWidth="1"/>
+    <col min="31" max="32" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -3444,190 +3411,196 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>306</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>307</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
-        <v>252</v>
-      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="AA1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="AC1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF1" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>271</v>
+      <c r="S2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="Y2" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="AB2" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="T3" t="s">
-        <v>260</v>
-      </c>
+      <c r="AF2" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="U3" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="V3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="W3" t="s">
-        <v>272</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+      <c r="X3" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -3647,101 +3620,104 @@
         <v>232</v>
       </c>
       <c r="G4" t="s">
+        <v>506</v>
+      </c>
+      <c r="H4" t="s">
+        <v>507</v>
+      </c>
+      <c r="I4" t="s">
+        <v>508</v>
+      </c>
+      <c r="J4" t="s">
         <v>233</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>234</v>
       </c>
-      <c r="I4" t="s">
-        <v>235</v>
-      </c>
-      <c r="J4" t="s">
-        <v>236</v>
-      </c>
-      <c r="K4" t="s">
-        <v>239</v>
-      </c>
       <c r="L4" t="s">
+        <v>237</v>
+      </c>
+      <c r="M4" t="s">
+        <v>240</v>
+      </c>
+      <c r="N4" t="s">
+        <v>241</v>
+      </c>
+      <c r="O4" t="s">
         <v>242</v>
       </c>
-      <c r="M4" t="s">
-        <v>243</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>244</v>
       </c>
-      <c r="O4" t="s">
-        <v>246</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
+        <v>247</v>
+      </c>
+      <c r="R4" t="s">
         <v>249</v>
       </c>
-      <c r="Q4" t="s">
-        <v>251</v>
-      </c>
-      <c r="R4" t="s">
-        <v>254</v>
-      </c>
       <c r="S4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="T4" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="U4" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="V4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="W4" t="s">
+        <v>267</v>
+      </c>
+      <c r="X4" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z4" t="s">
         <v>273</v>
       </c>
-      <c r="X4" t="s">
-        <v>274</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>275</v>
       </c>
-      <c r="Z4" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>278</v>
-      </c>
       <c r="AB4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AC4" t="s">
+        <v>280</v>
+      </c>
+      <c r="AD4" t="s">
         <v>223</v>
       </c>
-      <c r="AD4" t="s">
-        <v>283</v>
-      </c>
       <c r="AE4" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>484</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>480</v>
+        <v>471</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>467</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
-      <c r="AD6" t="s">
-        <v>501</v>
-      </c>
       <c r="AE6" t="s">
         <v>488</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -3751,10 +3727,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3766,231 +3742,181 @@
     <col min="5" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+    <col min="9" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="270" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>308</v>
+        <v>224</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>311</v>
+        <v>224</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>291</v>
+        <v>286</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="N2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
         <v>228</v>
       </c>
       <c r="C4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I4" t="s">
         <v>310</v>
       </c>
       <c r="J4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K4" t="s">
-        <v>316</v>
-      </c>
-      <c r="L4" t="s">
-        <v>319</v>
-      </c>
-      <c r="M4" t="s">
-        <v>322</v>
-      </c>
-      <c r="N4" t="s">
-        <v>323</v>
-      </c>
-      <c r="O4" t="s">
-        <v>324</v>
-      </c>
-      <c r="P4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>496</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>483</v>
       </c>
       <c r="B6" t="s">
+        <v>471</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="E6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>476</v>
+      </c>
+      <c r="J6" t="s">
+        <v>480</v>
+      </c>
+      <c r="K6" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="E6" t="s">
-        <v>295</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="B7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="E7" t="s">
+        <v>486</v>
+      </c>
+      <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="N6" t="s">
-        <v>489</v>
-      </c>
-      <c r="O6" t="s">
-        <v>493</v>
-      </c>
-      <c r="P6" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="B7" t="s">
-        <v>484</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="E7" t="s">
-        <v>499</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>489</v>
-      </c>
-      <c r="O7" t="s">
-        <v>493</v>
-      </c>
-      <c r="P7" t="s">
-        <v>500</v>
+      <c r="I7" t="s">
+        <v>476</v>
+      </c>
+      <c r="J7" t="s">
+        <v>480</v>
+      </c>
+      <c r="K7" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -4024,176 +3950,176 @@
     <col min="14" max="14" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="120" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="165" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>351</v>
+      <c r="J2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="I3" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="J3" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="K3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="M3" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="N3" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G4" t="s">
+        <v>345</v>
+      </c>
+      <c r="H4" t="s">
+        <v>346</v>
+      </c>
+      <c r="I4" t="s">
+        <v>349</v>
+      </c>
+      <c r="J4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K4" t="s">
+        <v>351</v>
+      </c>
+      <c r="L4" t="s">
         <v>353</v>
       </c>
-      <c r="C4" t="s">
+      <c r="M4" t="s">
         <v>354</v>
       </c>
-      <c r="D4" t="s">
+      <c r="N4" t="s">
         <v>355</v>
       </c>
-      <c r="E4" t="s">
-        <v>356</v>
-      </c>
-      <c r="F4" t="s">
-        <v>357</v>
-      </c>
-      <c r="G4" t="s">
-        <v>358</v>
-      </c>
-      <c r="H4" t="s">
-        <v>359</v>
-      </c>
-      <c r="I4" t="s">
-        <v>362</v>
-      </c>
-      <c r="J4" t="s">
-        <v>363</v>
-      </c>
-      <c r="K4" t="s">
-        <v>364</v>
-      </c>
-      <c r="L4" t="s">
-        <v>366</v>
-      </c>
-      <c r="M4" t="s">
-        <v>367</v>
-      </c>
-      <c r="N4" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="B6" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="G6" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="H6" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -4207,7 +4133,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4229,80 +4155,80 @@
         <v>224</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>337</v>
+      <c r="B2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>384</v>
+        <v>361</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="I3" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4310,50 +4236,50 @@
         <v>227</v>
       </c>
       <c r="B4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" t="s">
+        <v>360</v>
+      </c>
+      <c r="G4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" t="s">
+        <v>362</v>
+      </c>
+      <c r="I4" t="s">
+        <v>366</v>
+      </c>
+      <c r="J4" t="s">
         <v>369</v>
       </c>
-      <c r="C4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D4" t="s">
-        <v>371</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>372</v>
       </c>
-      <c r="F4" t="s">
-        <v>373</v>
-      </c>
-      <c r="G4" t="s">
-        <v>374</v>
-      </c>
-      <c r="H4" t="s">
-        <v>375</v>
-      </c>
-      <c r="I4" t="s">
-        <v>379</v>
-      </c>
-      <c r="J4" t="s">
-        <v>382</v>
-      </c>
-      <c r="K4" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="G6" t="s">
-        <v>503</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>504</v>
+        <v>490</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -4366,7 +4292,7 @@
   <dimension ref="A1:AS6"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+      <selection activeCell="X4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4420,494 +4346,494 @@
         <v>224</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>360</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="P2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>361</v>
-      </c>
       <c r="AB2" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH2" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="AC2" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="AI2" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>450</v>
-      </c>
       <c r="AR2" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>452</v>
+        <v>438</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="O3" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="P3" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="Q3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="S3" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="T3" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="U3" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="V3" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="W3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="Y3" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="Z3" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="AB3" t="s">
+        <v>412</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>419</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>336</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="AH4" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AI4" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="AM4" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="AE3" t="s">
-        <v>341</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>343</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>346</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>349</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>323</v>
-      </c>
-      <c r="B4" t="s">
-        <v>386</v>
-      </c>
-      <c r="C4" t="s">
-        <v>387</v>
-      </c>
-      <c r="D4" t="s">
-        <v>388</v>
-      </c>
-      <c r="E4" t="s">
-        <v>389</v>
-      </c>
-      <c r="F4" t="s">
-        <v>390</v>
-      </c>
-      <c r="G4" t="s">
-        <v>393</v>
-      </c>
-      <c r="H4" t="s">
-        <v>396</v>
-      </c>
-      <c r="I4" t="s">
-        <v>399</v>
-      </c>
-      <c r="J4" t="s">
-        <v>402</v>
-      </c>
-      <c r="K4" t="s">
-        <v>404</v>
-      </c>
-      <c r="L4" t="s">
-        <v>405</v>
-      </c>
-      <c r="M4" t="s">
-        <v>407</v>
-      </c>
-      <c r="N4" t="s">
-        <v>408</v>
-      </c>
-      <c r="O4" t="s">
-        <v>409</v>
-      </c>
-      <c r="P4" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>411</v>
-      </c>
-      <c r="R4" t="s">
-        <v>413</v>
-      </c>
-      <c r="S4" t="s">
-        <v>414</v>
-      </c>
-      <c r="T4" t="s">
-        <v>415</v>
-      </c>
-      <c r="U4" t="s">
-        <v>416</v>
-      </c>
-      <c r="V4" t="s">
-        <v>417</v>
-      </c>
-      <c r="W4" t="s">
-        <v>418</v>
-      </c>
-      <c r="X4" t="s">
-        <v>420</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>421</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>422</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>509</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>426</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>429</v>
-      </c>
-      <c r="AD4" t="s">
+      <c r="AN4" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AO4" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="AF4" t="s">
-        <v>435</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AP4" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AQ4" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="AR4" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AS4" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>440</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>443</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>444</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>445</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>446</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>447</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>449</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>450</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>451</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>452</v>
-      </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:45" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="K6" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="M6" t="s">
-        <v>491</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>505</v>
+        <v>478</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>492</v>
       </c>
       <c r="AA6" t="s">
-        <v>510</v>
-      </c>
-      <c r="AB6" s="5" t="s">
-        <v>492</v>
+        <v>497</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>479</v>
       </c>
       <c r="AC6" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="AD6" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>